<commit_message>
Working on RAD Implementation
</commit_message>
<xml_diff>
--- a/Documents/WPI_Airlines_Booking_T1_Backlog.xlsx
+++ b/Documents/WPI_Airlines_Booking_T1_Backlog.xlsx
@@ -1,43 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoarguelloserrano/WPI/Airlines-Project/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E2DDAE0-0A94-2C44-8720-0FC8A756A9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCE5609-1487-8E48-80BD-E458C7F80023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="7240" windowWidth="28040" windowHeight="17440" xr2:uid="{B0CACAD1-8886-C740-9EC7-1D41F121AE05}"/>
+    <workbookView xWindow="1980" yWindow="3320" windowWidth="31500" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Agency airline travel reservation system to a Retail Customer airline reservation system</t>
+  </si>
+  <si>
+    <t>Front_End</t>
+  </si>
+  <si>
+    <t>Back_End</t>
+  </si>
+  <si>
+    <t>DB_Admin</t>
+  </si>
+  <si>
+    <t>1. Application must access the data information tru and API [plain text]</t>
+  </si>
+  <si>
+    <t>2. App must allow client to to reserve travel from the destination airport to an arrival airport using a series of connecting flights with a maximum of two stopovers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. The App must verify that each stopover has sufficient time (layover time) to allow a passenger to transition from the gate of the arrival flight to the gate of the next departing flight before the departing flights leaves. </t>
+  </si>
+  <si>
+    <t>4. The App must verufy that layover time is also sufficient length to allow the airline to transfer the passenger’s bags from one flight to the next</t>
+  </si>
+  <si>
+    <t>5. The Front-End App must display the departure time and arrival time of each leg in airport local time. The server specifies flight times in GMT (Greenwich Mean Time.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. The Front-End must allow the user has the ability to reserve flights to travel either one-way (from departure to destination), or reserve a round-trip flight (from departure to destination and back to original departure airport.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. The Front-End must allow the user reserves either first class seating or coach seating for travel. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. The Front-End must verify The client software should properly behave in situations where requested seating is not available for all legs of the flight. </t>
+  </si>
+  <si>
+    <t>9. The Front-End must allow user to search for flights using departure date, arrival dates and respective time windows within each. The App will not offer flight choices with unreasonable layover times</t>
+  </si>
+  <si>
+    <t>10. The App must allow multiple users reserving fligths at same time.  To support concurrency, the server API will support locking of the database. When locked, only the client software which locked the database will be able to update the database. The database will prohibit changes when the database is not locked. Database locks, if not explicitly released, will be automatically released within a reasonable period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. The Front-end must display  flights sorted by price, departure time, arrival time or travel time. </t>
+  </si>
+  <si>
+    <t>Usability, to facilitate user selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. The Front-end must let the user confirm selection before the reservation is completed. </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,8 +113,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -161,26 +218,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -213,23 +253,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -372,24 +395,154 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45F3881-4701-6C4F-A8A0-CDD2D3DD3246}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="69" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Requirements table plus more changes
</commit_message>
<xml_diff>
--- a/Documents/WPI_Airlines_Booking_T1_Backlog.xlsx
+++ b/Documents/WPI_Airlines_Booking_T1_Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoarguelloserrano/WPI/Airlines-Project/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA17527F-6A3A-5448-A5DD-01CEA9A9C7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8DFF8A-1091-184F-91C9-2A587ACAF557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21900" yWindow="1100" windowWidth="32060" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10540" yWindow="6380" windowWidth="32060" windowHeight="23620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>